<commit_message>
Make _color is a required positional param Bug fix in `excelColor` getter, for detecting predefined material color Make test consistent
</commit_message>
<xml_diff>
--- a/test/test_resources/excel_default_sheet_removed_1.xlsx
+++ b/test/test_resources/excel_default_sheet_removed_1.xlsx
@@ -16,50 +16,32 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font/>
+    <font>
+      <color rgb="1F000000"/>
+    </font>
+    <font>
+      <color rgb="42000000"/>
+    </font>
+    <font>
+      <color rgb="61000000"/>
+    </font>
+    <font>
+      <color rgb="73000000"/>
+    </font>
   </fonts>
-  <fills count="26">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="lightGray"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF80AB"/>
-        <bgColor rgb="FFFF80AB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFDD835"/>
-        <bgColor rgb="FFFDD835"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7B1FA2"/>
-        <bgColor rgb="FF7B1FA2"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4E342E"/>
-        <bgColor rgb="FF4E342E"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -69,135 +51,139 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF2196F3"/>
-        <bgColor rgb="FF2196F3"/>
+        <fgColor rgb="FFE91E63"/>
+        <bgColor rgb="FFE91E63"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF90CAF9"/>
-        <bgColor rgb="FF90CAF9"/>
+        <fgColor rgb="FF9C27B0"/>
+        <bgColor rgb="FF9C27B0"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00BCD4"/>
-        <bgColor rgb="FF00BCD4"/>
+        <fgColor rgb="FF673AB7"/>
+        <bgColor rgb="FF673AB7"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFBE9E7"/>
-        <bgColor rgb="FFFBE9E7"/>
+        <fgColor rgb="FF3F51B5"/>
+        <bgColor rgb="FF3F51B5"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFAB00"/>
-        <bgColor rgb="FFFFAB00"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE57F"/>
-        <bgColor rgb="FFFFE57F"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF4DB6AC"/>
-        <bgColor rgb="FF4DB6AC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFAB91"/>
-        <bgColor rgb="FFFFAB91"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF84FFFF"/>
-        <bgColor rgb="FF84FFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF546E7A"/>
-        <bgColor rgb="FF546E7A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00E676"/>
-        <bgColor rgb="FF00E676"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC0CA33"/>
-        <bgColor rgb="FFC0CA33"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBA68C8"/>
-        <bgColor rgb="FFBA68C8"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF448AFF"/>
-        <bgColor rgb="FF448AFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF7986CB"/>
-        <bgColor rgb="FF7986CB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF5722"/>
-        <bgColor rgb="FFFF5722"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="6">
     <border/>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF5252"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF5252"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF5252"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF5252"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFFF4081"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFFF4081"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFFF4081"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFFF4081"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFE040FB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFE040FB"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFE040FB"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFE040FB"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7C4DFF"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7C4DFF"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7C4DFF"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7C4DFF"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF536DFE"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF536DFE"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF536DFE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF536DFE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="26">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="6" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="7" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="8" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="9" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="10" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="11" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="12" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="13" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="14" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="15" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="16" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="17" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="18" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="19" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="20" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="21" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="22" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="23" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="24" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf borderId="0" fillId="25" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="3" fillId="2" fontId="3" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="3" fillId="3" fontId="3" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="4" fillId="3" fontId="4" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="5" fillId="3" fontId="5" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="1" fillId="4" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="2" fillId="4" fontId="2" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="3" fillId="4" fontId="3" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="4" fillId="4" fontId="4" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="5" fillId="4" fontId="5" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="1" fillId="5" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="2" fillId="5" fontId="2" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="3" fillId="5" fontId="3" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="4" fillId="5" fontId="4" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="5" fillId="5" fontId="5" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="1" fillId="6" fontId="1" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="2" fillId="6" fontId="2" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="3" fillId="6" fontId="3" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="4" fillId="6" fontId="4" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf borderId="5" fillId="6" fontId="5" numFmtId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -413,87 +399,87 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C1" s="3">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D1" s="4">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E1" s="5">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="6">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="7">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C2" s="8">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="D2" s="9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="E2" s="10">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="11">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="12">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C3" s="13">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="D3" s="14">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="E3" s="15">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="16">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="17">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C4" s="18">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="D4" s="19">
-        <v>9</v>
-      </c>
-      <c r="E4" s="6">
-        <v>7</v>
+        <v>16</v>
+      </c>
+      <c r="E4" s="20">
+        <v>20</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="20">
-        <v>0</v>
-      </c>
-      <c r="B5" s="21">
-        <v>4</v>
-      </c>
-      <c r="C5" s="22">
-        <v>6</v>
-      </c>
-      <c r="D5" s="23">
-        <v>12</v>
-      </c>
-      <c r="E5" s="24">
-        <v>8</v>
+      <c r="A5" s="21">
+        <v>5</v>
+      </c>
+      <c r="B5" s="22">
+        <v>10</v>
+      </c>
+      <c r="C5" s="23">
+        <v>15</v>
+      </c>
+      <c r="D5" s="24">
+        <v>20</v>
+      </c>
+      <c r="E5" s="25">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>